<commit_message>
Fixed bugs, corrected startup procedure, improved database class
</commit_message>
<xml_diff>
--- a/Test Data/Claims/1.xlsx
+++ b/Test Data/Claims/1.xlsx
@@ -333,8 +333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F10:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -367,6 +367,9 @@
       <c r="F13">
         <v>4</v>
       </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.55000000000000004">
       <c r="F14">

</xml_diff>